<commit_message>
2025.01.04_2 deleted obsolete tidyverse part from the end
</commit_message>
<xml_diff>
--- a/data_codebook.xlsx
+++ b/data_codebook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavosplmoura/Library/Mobile Documents/com~apple~CloudDocs/Medicina/Biblioteca/Research/Data Science/Data Science/PROJECTS/DVEP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664BD572-A1A2-DF46-BA88-D9D4889D2C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809C7A70-B402-C84A-B6D7-DBC4C011C2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{64E364A7-669F-4B4E-A75E-FD8B217DB5CF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10123" uniqueCount="5732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10125" uniqueCount="5733">
   <si>
     <t>variable</t>
   </si>
@@ -17514,10 +17514,13 @@
     <t>k</t>
   </si>
   <si>
-    <t>eleg_arm_1, 0 | 1visit_arm_1, 1 |2visit_arm_1, 2 | 3visit_arm_1, 3</t>
-  </si>
-  <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>eleg_arm_1, 0 | 1visit_arm_1, 1 | 2visit_arm_1, 2 | 3visit_arm_1, 3</t>
   </si>
 </sst>
 </file>
@@ -18230,6 +18233,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C9BD1FE7-06E6-AF49-9672-E4E31AED68CC}" name="Table2" displayName="Table2" ref="A1:AA781" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A1:AA781" xr:uid="{C9BD1FE7-06E6-AF49-9672-E4E31AED68CC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA781">
+    <sortCondition ref="A1:A781"/>
+  </sortState>
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{204E05AD-B324-584D-9052-1D5D7A5AF23C}" name="index" dataDxfId="30"/>
     <tableColumn id="2" xr3:uid="{E78D0B38-AC8A-0541-A7D9-8D9DE8100BFC}" name="variable" dataDxfId="29"/>
@@ -18582,9 +18588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{647B9358-69AB-914B-A705-A7628698E265}">
   <dimension ref="A1:AA781"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="178" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="163" zoomScaleNormal="178" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -18599,7 +18605,7 @@
     <col min="10" max="10" width="13.19921875" customWidth="1"/>
     <col min="11" max="11" width="6.796875" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="99.796875" customWidth="1"/>
+    <col min="13" max="13" width="28.59765625" customWidth="1"/>
     <col min="15" max="15" width="34.3984375" customWidth="1"/>
     <col min="17" max="17" width="53.59765625" customWidth="1"/>
     <col min="18" max="18" width="8.19921875" customWidth="1"/>
@@ -18787,7 +18793,7 @@
         <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>5730</v>
+        <v>5732</v>
       </c>
       <c r="N3" t="s">
         <v>38</v>
@@ -19073,7 +19079,7 @@
         <v>72</v>
       </c>
       <c r="L8" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M8" t="s">
         <v>73</v>
@@ -19138,7 +19144,7 @@
         <v>72</v>
       </c>
       <c r="L9" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M9" t="s">
         <v>80</v>
@@ -19203,7 +19209,7 @@
         <v>72</v>
       </c>
       <c r="L10" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M10" t="s">
         <v>90</v>
@@ -19265,7 +19271,7 @@
         <v>72</v>
       </c>
       <c r="L11" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M11" t="s">
         <v>99</v>
@@ -19327,7 +19333,7 @@
         <v>72</v>
       </c>
       <c r="L12" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M12" t="s">
         <v>108</v>
@@ -19389,7 +19395,7 @@
         <v>72</v>
       </c>
       <c r="L13" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M13" t="s">
         <v>116</v>
@@ -19451,7 +19457,7 @@
         <v>72</v>
       </c>
       <c r="L14" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M14" t="s">
         <v>125</v>
@@ -19566,7 +19572,7 @@
         <v>72</v>
       </c>
       <c r="L16" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M16" t="s">
         <v>140</v>
@@ -19631,7 +19637,7 @@
         <v>72</v>
       </c>
       <c r="L17" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M17" t="s">
         <v>125</v>
@@ -19879,7 +19885,7 @@
         <v>72</v>
       </c>
       <c r="L21" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M21" t="s">
         <v>125</v>
@@ -19997,7 +20003,7 @@
         <v>72</v>
       </c>
       <c r="L23" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M23" t="s">
         <v>125</v>
@@ -20115,7 +20121,7 @@
         <v>72</v>
       </c>
       <c r="L25" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M25" t="s">
         <v>125</v>
@@ -20177,7 +20183,7 @@
         <v>72</v>
       </c>
       <c r="L26" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M26" t="s">
         <v>125</v>
@@ -20239,7 +20245,7 @@
         <v>72</v>
       </c>
       <c r="L27" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M27" t="s">
         <v>125</v>
@@ -20301,7 +20307,7 @@
         <v>72</v>
       </c>
       <c r="L28" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M28" t="s">
         <v>125</v>
@@ -20363,7 +20369,7 @@
         <v>72</v>
       </c>
       <c r="L29" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M29" t="s">
         <v>125</v>
@@ -20425,7 +20431,7 @@
         <v>72</v>
       </c>
       <c r="L30" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M30" t="s">
         <v>125</v>
@@ -20487,7 +20493,7 @@
         <v>72</v>
       </c>
       <c r="L31" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M31" t="s">
         <v>125</v>
@@ -20549,7 +20555,7 @@
         <v>72</v>
       </c>
       <c r="L32" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M32" t="s">
         <v>125</v>
@@ -20611,7 +20617,7 @@
         <v>72</v>
       </c>
       <c r="L33" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M33" t="s">
         <v>125</v>
@@ -20673,7 +20679,7 @@
         <v>72</v>
       </c>
       <c r="L34" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M34" t="s">
         <v>125</v>
@@ -20735,7 +20741,7 @@
         <v>72</v>
       </c>
       <c r="L35" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M35" t="s">
         <v>125</v>
@@ -20797,7 +20803,7 @@
         <v>72</v>
       </c>
       <c r="L36" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M36" t="s">
         <v>125</v>
@@ -20859,7 +20865,7 @@
         <v>72</v>
       </c>
       <c r="L37" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M37" t="s">
         <v>125</v>
@@ -20924,7 +20930,7 @@
         <v>72</v>
       </c>
       <c r="L38" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M38" t="s">
         <v>125</v>
@@ -20986,7 +20992,7 @@
         <v>72</v>
       </c>
       <c r="L39" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M39" t="s">
         <v>125</v>
@@ -21048,7 +21054,7 @@
         <v>72</v>
       </c>
       <c r="L40" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M40" t="s">
         <v>125</v>
@@ -21110,7 +21116,7 @@
         <v>72</v>
       </c>
       <c r="L41" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M41" t="s">
         <v>125</v>
@@ -21172,7 +21178,7 @@
         <v>72</v>
       </c>
       <c r="L42" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M42" t="s">
         <v>125</v>
@@ -21234,7 +21240,7 @@
         <v>72</v>
       </c>
       <c r="L43" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M43" t="s">
         <v>125</v>
@@ -21296,7 +21302,7 @@
         <v>72</v>
       </c>
       <c r="L44" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M44" t="s">
         <v>125</v>
@@ -21358,7 +21364,7 @@
         <v>72</v>
       </c>
       <c r="L45" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M45" t="s">
         <v>125</v>
@@ -21420,7 +21426,7 @@
         <v>72</v>
       </c>
       <c r="L46" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M46" t="s">
         <v>125</v>
@@ -21482,7 +21488,7 @@
         <v>72</v>
       </c>
       <c r="L47" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M47" t="s">
         <v>125</v>
@@ -21544,7 +21550,7 @@
         <v>72</v>
       </c>
       <c r="L48" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M48" t="s">
         <v>125</v>
@@ -21606,7 +21612,7 @@
         <v>72</v>
       </c>
       <c r="L49" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M49" t="s">
         <v>125</v>
@@ -21668,7 +21674,7 @@
         <v>72</v>
       </c>
       <c r="L50" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M50" t="s">
         <v>125</v>
@@ -21730,7 +21736,7 @@
         <v>72</v>
       </c>
       <c r="L51" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M51" t="s">
         <v>125</v>
@@ -22019,7 +22025,7 @@
         <v>72</v>
       </c>
       <c r="L56" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M56" t="s">
         <v>423</v>
@@ -22081,7 +22087,7 @@
         <v>432</v>
       </c>
       <c r="L57" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M57" t="s">
         <v>125</v>
@@ -22143,7 +22149,7 @@
         <v>432</v>
       </c>
       <c r="L58" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M58" t="s">
         <v>125</v>
@@ -22205,7 +22211,7 @@
         <v>432</v>
       </c>
       <c r="L59" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M59" t="s">
         <v>125</v>
@@ -22267,7 +22273,7 @@
         <v>72</v>
       </c>
       <c r="L60" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M60" t="s">
         <v>125</v>
@@ -22329,7 +22335,7 @@
         <v>72</v>
       </c>
       <c r="L61" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M61" t="s">
         <v>465</v>
@@ -22450,7 +22456,7 @@
         <v>72</v>
       </c>
       <c r="L63" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M63" t="s">
         <v>125</v>
@@ -22515,7 +22521,7 @@
         <v>72</v>
       </c>
       <c r="L64" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M64" t="s">
         <v>125</v>
@@ -22639,7 +22645,7 @@
         <v>72</v>
       </c>
       <c r="L66" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M66" t="s">
         <v>125</v>
@@ -22701,7 +22707,7 @@
         <v>72</v>
       </c>
       <c r="L67" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M67" t="s">
         <v>125</v>
@@ -22763,7 +22769,7 @@
         <v>72</v>
       </c>
       <c r="L68" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M68" t="s">
         <v>125</v>
@@ -22878,7 +22884,7 @@
         <v>72</v>
       </c>
       <c r="L70" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M70" t="s">
         <v>125</v>
@@ -22940,7 +22946,7 @@
         <v>72</v>
       </c>
       <c r="L71" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M71" t="s">
         <v>125</v>
@@ -23058,7 +23064,7 @@
         <v>72</v>
       </c>
       <c r="L73" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M73" t="s">
         <v>125</v>
@@ -23120,7 +23126,7 @@
         <v>72</v>
       </c>
       <c r="L74" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M74" t="s">
         <v>557</v>
@@ -23182,7 +23188,7 @@
         <v>28</v>
       </c>
       <c r="L75" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="P75" t="s">
         <v>566</v>
@@ -23297,7 +23303,7 @@
         <v>72</v>
       </c>
       <c r="L77" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M77" t="s">
         <v>578</v>
@@ -23359,7 +23365,7 @@
         <v>72</v>
       </c>
       <c r="L78" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M78" t="s">
         <v>125</v>
@@ -23551,7 +23557,7 @@
         <v>72</v>
       </c>
       <c r="L81" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M81" t="s">
         <v>578</v>
@@ -23970,7 +23976,7 @@
         <v>72</v>
       </c>
       <c r="L88" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M88" t="s">
         <v>664</v>
@@ -24088,7 +24094,7 @@
         <v>72</v>
       </c>
       <c r="L90" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M90" t="s">
         <v>578</v>
@@ -24150,7 +24156,7 @@
         <v>28</v>
       </c>
       <c r="L91" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="Q91" t="s">
         <v>567</v>
@@ -24206,7 +24212,7 @@
         <v>72</v>
       </c>
       <c r="L92" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M92" t="s">
         <v>693</v>
@@ -24271,7 +24277,7 @@
         <v>72</v>
       </c>
       <c r="L93" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M93" t="s">
         <v>702</v>
@@ -24336,7 +24342,7 @@
         <v>72</v>
       </c>
       <c r="L94" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M94" t="s">
         <v>711</v>
@@ -24401,7 +24407,7 @@
         <v>72</v>
       </c>
       <c r="L95" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M95" t="s">
         <v>711</v>
@@ -24466,7 +24472,7 @@
         <v>72</v>
       </c>
       <c r="L96" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M96" t="s">
         <v>711</v>
@@ -24531,7 +24537,7 @@
         <v>72</v>
       </c>
       <c r="L97" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M97" t="s">
         <v>711</v>
@@ -24596,7 +24602,7 @@
         <v>72</v>
       </c>
       <c r="L98" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M98" t="s">
         <v>711</v>
@@ -24661,7 +24667,7 @@
         <v>72</v>
       </c>
       <c r="L99" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M99" t="s">
         <v>711</v>
@@ -24726,7 +24732,7 @@
         <v>72</v>
       </c>
       <c r="L100" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M100" t="s">
         <v>711</v>
@@ -24791,7 +24797,7 @@
         <v>72</v>
       </c>
       <c r="L101" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M101" t="s">
         <v>768</v>
@@ -24856,7 +24862,7 @@
         <v>72</v>
       </c>
       <c r="L102" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M102" t="s">
         <v>768</v>
@@ -24921,7 +24927,7 @@
         <v>72</v>
       </c>
       <c r="L103" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M103" t="s">
         <v>768</v>
@@ -24986,7 +24992,7 @@
         <v>72</v>
       </c>
       <c r="L104" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M104" t="s">
         <v>768</v>
@@ -25051,7 +25057,7 @@
         <v>72</v>
       </c>
       <c r="L105" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M105" t="s">
         <v>768</v>
@@ -25116,7 +25122,7 @@
         <v>72</v>
       </c>
       <c r="L106" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M106" t="s">
         <v>693</v>
@@ -25181,7 +25187,7 @@
         <v>72</v>
       </c>
       <c r="L107" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M107" t="s">
         <v>693</v>
@@ -25246,7 +25252,7 @@
         <v>72</v>
       </c>
       <c r="L108" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M108" t="s">
         <v>693</v>
@@ -25311,7 +25317,7 @@
         <v>72</v>
       </c>
       <c r="L109" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M109" t="s">
         <v>693</v>
@@ -25376,7 +25382,7 @@
         <v>72</v>
       </c>
       <c r="L110" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M110" t="s">
         <v>693</v>
@@ -25441,7 +25447,7 @@
         <v>72</v>
       </c>
       <c r="L111" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M111" t="s">
         <v>693</v>
@@ -25506,7 +25512,7 @@
         <v>72</v>
       </c>
       <c r="L112" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M112" t="s">
         <v>693</v>
@@ -25571,7 +25577,7 @@
         <v>72</v>
       </c>
       <c r="L113" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M113" t="s">
         <v>693</v>
@@ -25636,7 +25642,7 @@
         <v>72</v>
       </c>
       <c r="L114" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M114" t="s">
         <v>693</v>
@@ -25701,7 +25707,7 @@
         <v>72</v>
       </c>
       <c r="L115" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M115" t="s">
         <v>693</v>
@@ -25766,7 +25772,7 @@
         <v>72</v>
       </c>
       <c r="L116" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M116" t="s">
         <v>693</v>
@@ -25831,7 +25837,7 @@
         <v>72</v>
       </c>
       <c r="L117" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M117" t="s">
         <v>896</v>
@@ -25896,7 +25902,7 @@
         <v>72</v>
       </c>
       <c r="L118" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M118" t="s">
         <v>905</v>
@@ -26406,7 +26412,7 @@
         <v>72</v>
       </c>
       <c r="L127" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M127" t="s">
         <v>578</v>
@@ -26468,7 +26474,7 @@
         <v>28</v>
       </c>
       <c r="L128" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="Q128" t="s">
         <v>567</v>
@@ -26524,7 +26530,7 @@
         <v>72</v>
       </c>
       <c r="L129" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M129" t="s">
         <v>981</v>
@@ -26589,7 +26595,7 @@
         <v>72</v>
       </c>
       <c r="L130" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M130" t="s">
         <v>981</v>
@@ -26654,7 +26660,7 @@
         <v>72</v>
       </c>
       <c r="L131" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M131" t="s">
         <v>981</v>
@@ -26719,7 +26725,7 @@
         <v>72</v>
       </c>
       <c r="L132" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M132" t="s">
         <v>981</v>
@@ -26784,7 +26790,7 @@
         <v>72</v>
       </c>
       <c r="L133" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M133" t="s">
         <v>981</v>
@@ -26849,7 +26855,7 @@
         <v>72</v>
       </c>
       <c r="L134" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M134" t="s">
         <v>981</v>
@@ -26914,7 +26920,7 @@
         <v>72</v>
       </c>
       <c r="L135" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M135" t="s">
         <v>981</v>
@@ -26979,7 +26985,7 @@
         <v>72</v>
       </c>
       <c r="L136" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M136" t="s">
         <v>981</v>
@@ -27044,7 +27050,7 @@
         <v>72</v>
       </c>
       <c r="L137" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M137" t="s">
         <v>981</v>
@@ -27109,7 +27115,7 @@
         <v>72</v>
       </c>
       <c r="L138" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M138" t="s">
         <v>981</v>
@@ -27174,7 +27180,7 @@
         <v>72</v>
       </c>
       <c r="L139" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M139" t="s">
         <v>981</v>
@@ -27239,7 +27245,7 @@
         <v>72</v>
       </c>
       <c r="L140" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M140" t="s">
         <v>981</v>
@@ -27304,7 +27310,7 @@
         <v>72</v>
       </c>
       <c r="L141" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M141" t="s">
         <v>981</v>
@@ -27369,7 +27375,7 @@
         <v>72</v>
       </c>
       <c r="L142" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M142" t="s">
         <v>981</v>
@@ -27434,7 +27440,7 @@
         <v>72</v>
       </c>
       <c r="L143" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M143" t="s">
         <v>981</v>
@@ -27499,7 +27505,7 @@
         <v>72</v>
       </c>
       <c r="L144" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M144" t="s">
         <v>981</v>
@@ -27564,7 +27570,7 @@
         <v>72</v>
       </c>
       <c r="L145" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M145" t="s">
         <v>981</v>
@@ -27629,7 +27635,7 @@
         <v>72</v>
       </c>
       <c r="L146" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M146" t="s">
         <v>981</v>
@@ -27694,7 +27700,7 @@
         <v>72</v>
       </c>
       <c r="L147" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M147" t="s">
         <v>981</v>
@@ -27759,7 +27765,7 @@
         <v>72</v>
       </c>
       <c r="L148" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M148" t="s">
         <v>981</v>
@@ -27824,7 +27830,7 @@
         <v>72</v>
       </c>
       <c r="L149" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M149" t="s">
         <v>981</v>
@@ -28113,7 +28119,7 @@
         <v>72</v>
       </c>
       <c r="L154" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M154" t="s">
         <v>578</v>
@@ -28175,7 +28181,7 @@
         <v>28</v>
       </c>
       <c r="L155" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="Q155" t="s">
         <v>567</v>
@@ -28231,7 +28237,7 @@
         <v>72</v>
       </c>
       <c r="L156" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M156" t="s">
         <v>1188</v>
@@ -28296,7 +28302,7 @@
         <v>72</v>
       </c>
       <c r="L157" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M157" t="s">
         <v>1195</v>
@@ -28361,7 +28367,7 @@
         <v>72</v>
       </c>
       <c r="L158" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M158" t="s">
         <v>1202</v>
@@ -28426,7 +28432,7 @@
         <v>72</v>
       </c>
       <c r="L159" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M159" t="s">
         <v>1209</v>
@@ -28491,7 +28497,7 @@
         <v>72</v>
       </c>
       <c r="L160" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M160" t="s">
         <v>1216</v>
@@ -28556,7 +28562,7 @@
         <v>72</v>
       </c>
       <c r="L161" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M161" t="s">
         <v>1223</v>
@@ -28621,7 +28627,7 @@
         <v>72</v>
       </c>
       <c r="L162" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M162" t="s">
         <v>1230</v>
@@ -28686,7 +28692,7 @@
         <v>72</v>
       </c>
       <c r="L163" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M163" t="s">
         <v>1237</v>
@@ -28751,7 +28757,7 @@
         <v>72</v>
       </c>
       <c r="L164" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M164" t="s">
         <v>1244</v>
@@ -28816,7 +28822,7 @@
         <v>72</v>
       </c>
       <c r="L165" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M165" t="s">
         <v>1251</v>
@@ -28881,7 +28887,7 @@
         <v>72</v>
       </c>
       <c r="L166" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M166" t="s">
         <v>1258</v>
@@ -28946,7 +28952,7 @@
         <v>72</v>
       </c>
       <c r="L167" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M167" t="s">
         <v>1265</v>
@@ -29011,7 +29017,7 @@
         <v>72</v>
       </c>
       <c r="L168" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M168" t="s">
         <v>1272</v>
@@ -29076,7 +29082,7 @@
         <v>72</v>
       </c>
       <c r="L169" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M169" t="s">
         <v>1279</v>
@@ -29141,7 +29147,7 @@
         <v>72</v>
       </c>
       <c r="L170" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M170" t="s">
         <v>1286</v>
@@ -29206,7 +29212,7 @@
         <v>72</v>
       </c>
       <c r="L171" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M171" t="s">
         <v>1293</v>
@@ -30392,7 +30398,7 @@
         <v>72</v>
       </c>
       <c r="L191" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M191" t="s">
         <v>578</v>
@@ -31796,7 +31802,7 @@
         <v>72</v>
       </c>
       <c r="L215" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M215" t="s">
         <v>578</v>
@@ -31858,7 +31864,7 @@
         <v>28</v>
       </c>
       <c r="L216" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="Q216" t="s">
         <v>567</v>
@@ -32516,7 +32522,7 @@
         <v>72</v>
       </c>
       <c r="L227" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M227" t="s">
         <v>578</v>
@@ -32578,7 +32584,7 @@
         <v>28</v>
       </c>
       <c r="L228" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="Q228" t="s">
         <v>567</v>
@@ -34615,7 +34621,7 @@
         <v>432</v>
       </c>
       <c r="L261" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M261" t="s">
         <v>125</v>
@@ -34680,7 +34686,7 @@
         <v>72</v>
       </c>
       <c r="L262" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M262" t="s">
         <v>578</v>
@@ -34795,7 +34801,7 @@
         <v>28</v>
       </c>
       <c r="L264" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="Q264" t="s">
         <v>567</v>
@@ -34916,7 +34922,7 @@
         <v>72</v>
       </c>
       <c r="L266" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M266" t="s">
         <v>125</v>
@@ -34984,7 +34990,7 @@
         <v>72</v>
       </c>
       <c r="L267" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M267" t="s">
         <v>125</v>
@@ -35052,7 +35058,7 @@
         <v>72</v>
       </c>
       <c r="L268" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M268" t="s">
         <v>125</v>
@@ -35120,7 +35126,7 @@
         <v>72</v>
       </c>
       <c r="L269" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M269" t="s">
         <v>125</v>
@@ -35256,7 +35262,7 @@
         <v>72</v>
       </c>
       <c r="L271" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M271" t="s">
         <v>125</v>
@@ -35324,7 +35330,7 @@
         <v>72</v>
       </c>
       <c r="L272" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M272" t="s">
         <v>125</v>
@@ -35392,7 +35398,7 @@
         <v>72</v>
       </c>
       <c r="L273" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M273" t="s">
         <v>125</v>
@@ -35460,7 +35466,7 @@
         <v>72</v>
       </c>
       <c r="L274" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M274" t="s">
         <v>125</v>
@@ -35528,7 +35534,7 @@
         <v>72</v>
       </c>
       <c r="L275" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M275" t="s">
         <v>125</v>
@@ -35596,7 +35602,7 @@
         <v>28</v>
       </c>
       <c r="L276" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="Q276" t="s">
         <v>1974</v>
@@ -35658,7 +35664,7 @@
         <v>28</v>
       </c>
       <c r="L277" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="Q277" t="s">
         <v>1974</v>
@@ -35720,7 +35726,7 @@
         <v>72</v>
       </c>
       <c r="L278" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M278" t="s">
         <v>125</v>
@@ -35788,7 +35794,7 @@
         <v>28</v>
       </c>
       <c r="L279" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="Q279" t="s">
         <v>1974</v>
@@ -36346,7 +36352,7 @@
         <v>432</v>
       </c>
       <c r="L288" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M288" t="s">
         <v>125</v>
@@ -36411,7 +36417,7 @@
         <v>72</v>
       </c>
       <c r="L289" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M289" t="s">
         <v>578</v>
@@ -36473,7 +36479,7 @@
         <v>72</v>
       </c>
       <c r="L290" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M290" t="s">
         <v>125</v>
@@ -36535,7 +36541,7 @@
         <v>72</v>
       </c>
       <c r="L291" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M291" t="s">
         <v>2078</v>
@@ -36600,7 +36606,7 @@
         <v>72</v>
       </c>
       <c r="L292" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M292" t="s">
         <v>125</v>
@@ -36662,7 +36668,7 @@
         <v>72</v>
       </c>
       <c r="L293" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M293" t="s">
         <v>125</v>
@@ -36724,7 +36730,7 @@
         <v>72</v>
       </c>
       <c r="L294" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M294" t="s">
         <v>125</v>
@@ -36786,7 +36792,7 @@
         <v>72</v>
       </c>
       <c r="L295" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M295" t="s">
         <v>125</v>
@@ -36848,7 +36854,7 @@
         <v>72</v>
       </c>
       <c r="L296" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M296" t="s">
         <v>125</v>
@@ -36910,7 +36916,7 @@
         <v>72</v>
       </c>
       <c r="L297" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M297" t="s">
         <v>125</v>
@@ -36972,7 +36978,7 @@
         <v>72</v>
       </c>
       <c r="L298" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M298" t="s">
         <v>125</v>
@@ -37034,7 +37040,7 @@
         <v>72</v>
       </c>
       <c r="L299" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M299" t="s">
         <v>125</v>
@@ -37096,7 +37102,7 @@
         <v>72</v>
       </c>
       <c r="L300" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M300" t="s">
         <v>125</v>
@@ -37158,7 +37164,7 @@
         <v>72</v>
       </c>
       <c r="L301" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M301" t="s">
         <v>125</v>
@@ -37220,7 +37226,7 @@
         <v>72</v>
       </c>
       <c r="L302" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M302" t="s">
         <v>125</v>
@@ -37282,7 +37288,7 @@
         <v>72</v>
       </c>
       <c r="L303" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M303" t="s">
         <v>125</v>
@@ -37344,7 +37350,7 @@
         <v>432</v>
       </c>
       <c r="L304" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M304" t="s">
         <v>2171</v>
@@ -37412,7 +37418,7 @@
         <v>432</v>
       </c>
       <c r="L305" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M305" t="s">
         <v>2181</v>
@@ -37480,7 +37486,7 @@
         <v>432</v>
       </c>
       <c r="L306" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M306" t="s">
         <v>2190</v>
@@ -37548,7 +37554,7 @@
         <v>432</v>
       </c>
       <c r="L307" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M307" t="s">
         <v>2199</v>
@@ -37616,7 +37622,7 @@
         <v>432</v>
       </c>
       <c r="L308" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M308" t="s">
         <v>2207</v>
@@ -37684,7 +37690,7 @@
         <v>72</v>
       </c>
       <c r="L309" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M309" t="s">
         <v>125</v>
@@ -37752,7 +37758,7 @@
         <v>432</v>
       </c>
       <c r="L310" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M310" t="s">
         <v>125</v>
@@ -37820,7 +37826,7 @@
         <v>72</v>
       </c>
       <c r="L311" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M311" t="s">
         <v>125</v>
@@ -39188,7 +39194,7 @@
         <v>432</v>
       </c>
       <c r="L332" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M332" t="s">
         <v>125</v>
@@ -39250,7 +39256,7 @@
         <v>72</v>
       </c>
       <c r="L333" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M333" t="s">
         <v>578</v>
@@ -39856,7 +39862,7 @@
         <v>72</v>
       </c>
       <c r="L342" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M342" t="s">
         <v>578</v>
@@ -40527,7 +40533,7 @@
         <v>72</v>
       </c>
       <c r="L352" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M352" t="s">
         <v>578</v>
@@ -40589,7 +40595,7 @@
         <v>72</v>
       </c>
       <c r="L353" t="s">
-        <v>49</v>
+        <v>5728</v>
       </c>
       <c r="M353" t="s">
         <v>2564</v>
@@ -40654,7 +40660,7 @@
         <v>72</v>
       </c>
       <c r="L354" t="s">
-        <v>49</v>
+        <v>5728</v>
       </c>
       <c r="M354" t="s">
         <v>2573</v>
@@ -40781,7 +40787,7 @@
         <v>432</v>
       </c>
       <c r="L356" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M356" t="s">
         <v>2588</v>
@@ -40855,7 +40861,7 @@
         <v>432</v>
       </c>
       <c r="L357" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M357" t="s">
         <v>2599</v>
@@ -40929,7 +40935,7 @@
         <v>432</v>
       </c>
       <c r="L358" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M358" t="s">
         <v>2599</v>
@@ -41053,7 +41059,7 @@
         <v>72</v>
       </c>
       <c r="L360" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M360" t="s">
         <v>578</v>
@@ -41115,7 +41121,7 @@
         <v>72</v>
       </c>
       <c r="L361" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M361" t="s">
         <v>2630</v>
@@ -41180,7 +41186,7 @@
         <v>72</v>
       </c>
       <c r="L362" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M362" t="s">
         <v>2640</v>
@@ -41248,7 +41254,7 @@
         <v>72</v>
       </c>
       <c r="L363" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M363" t="s">
         <v>2650</v>
@@ -41316,7 +41322,7 @@
         <v>72</v>
       </c>
       <c r="L364" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M364" t="s">
         <v>125</v>
@@ -41378,7 +41384,7 @@
         <v>72</v>
       </c>
       <c r="L365" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M365" t="s">
         <v>125</v>
@@ -41440,7 +41446,7 @@
         <v>72</v>
       </c>
       <c r="L366" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M366" t="s">
         <v>125</v>
@@ -41502,7 +41508,7 @@
         <v>72</v>
       </c>
       <c r="L367" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M367" t="s">
         <v>125</v>
@@ -41564,7 +41570,7 @@
         <v>72</v>
       </c>
       <c r="L368" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M368" t="s">
         <v>125</v>
@@ -41626,7 +41632,7 @@
         <v>72</v>
       </c>
       <c r="L369" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M369" t="s">
         <v>125</v>
@@ -41688,7 +41694,7 @@
         <v>72</v>
       </c>
       <c r="L370" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M370" t="s">
         <v>125</v>
@@ -41750,7 +41756,7 @@
         <v>72</v>
       </c>
       <c r="L371" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M371" t="s">
         <v>125</v>
@@ -41812,7 +41818,7 @@
         <v>72</v>
       </c>
       <c r="L372" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M372" t="s">
         <v>125</v>
@@ -41874,7 +41880,7 @@
         <v>72</v>
       </c>
       <c r="L373" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M373" t="s">
         <v>125</v>
@@ -42556,7 +42562,7 @@
         <v>72</v>
       </c>
       <c r="L384" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M384" t="s">
         <v>578</v>
@@ -42618,7 +42624,7 @@
         <v>72</v>
       </c>
       <c r="L385" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M385" t="s">
         <v>2812</v>
@@ -42975,7 +42981,7 @@
         <v>72</v>
       </c>
       <c r="L391" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M391" t="s">
         <v>578</v>
@@ -43037,7 +43043,7 @@
         <v>28</v>
       </c>
       <c r="L392" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="P392" t="s">
         <v>2862</v>
@@ -43096,7 +43102,7 @@
         <v>28</v>
       </c>
       <c r="L393" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="P393" t="s">
         <v>2862</v>
@@ -43155,7 +43161,7 @@
         <v>28</v>
       </c>
       <c r="L394" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="P394" t="s">
         <v>2862</v>
@@ -43214,7 +43220,7 @@
         <v>28</v>
       </c>
       <c r="L395" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="P395" t="s">
         <v>2862</v>
@@ -43273,7 +43279,7 @@
         <v>28</v>
       </c>
       <c r="L396" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="P396" t="s">
         <v>2862</v>
@@ -43332,7 +43338,7 @@
         <v>28</v>
       </c>
       <c r="L397" t="s">
-        <v>1714</v>
+        <v>5731</v>
       </c>
       <c r="P397" t="s">
         <v>2862</v>
@@ -44119,7 +44125,7 @@
         <v>72</v>
       </c>
       <c r="L411" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M411" t="s">
         <v>578</v>
@@ -44181,7 +44187,7 @@
         <v>72</v>
       </c>
       <c r="L412" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M412" t="s">
         <v>125</v>
@@ -44243,7 +44249,7 @@
         <v>72</v>
       </c>
       <c r="L413" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M413" t="s">
         <v>125</v>
@@ -44305,7 +44311,7 @@
         <v>72</v>
       </c>
       <c r="L414" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M414" t="s">
         <v>125</v>
@@ -44367,7 +44373,7 @@
         <v>72</v>
       </c>
       <c r="L415" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M415" t="s">
         <v>125</v>
@@ -44429,7 +44435,7 @@
         <v>72</v>
       </c>
       <c r="L416" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M416" t="s">
         <v>125</v>
@@ -44491,7 +44497,7 @@
         <v>72</v>
       </c>
       <c r="L417" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M417" t="s">
         <v>125</v>
@@ -44553,7 +44559,7 @@
         <v>72</v>
       </c>
       <c r="L418" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M418" t="s">
         <v>125</v>
@@ -44615,7 +44621,7 @@
         <v>72</v>
       </c>
       <c r="L419" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M419" t="s">
         <v>125</v>
@@ -44677,7 +44683,7 @@
         <v>72</v>
       </c>
       <c r="L420" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M420" t="s">
         <v>125</v>
@@ -44739,7 +44745,7 @@
         <v>72</v>
       </c>
       <c r="L421" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M421" t="s">
         <v>125</v>
@@ -44801,7 +44807,7 @@
         <v>72</v>
       </c>
       <c r="L422" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M422" t="s">
         <v>125</v>
@@ -44863,7 +44869,7 @@
         <v>72</v>
       </c>
       <c r="L423" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M423" t="s">
         <v>125</v>
@@ -47928,7 +47934,7 @@
         <v>72</v>
       </c>
       <c r="L475" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M475" t="s">
         <v>578</v>
@@ -47990,7 +47996,7 @@
         <v>72</v>
       </c>
       <c r="L476" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M476" t="s">
         <v>125</v>
@@ -48114,7 +48120,7 @@
         <v>72</v>
       </c>
       <c r="L478" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M478" t="s">
         <v>125</v>
@@ -48240,6 +48246,9 @@
       <c r="K480" t="s">
         <v>28</v>
       </c>
+      <c r="L480" t="s">
+        <v>1714</v>
+      </c>
       <c r="P480" t="s">
         <v>3437</v>
       </c>
@@ -48361,6 +48370,9 @@
       <c r="K482" t="s">
         <v>28</v>
       </c>
+      <c r="L482" t="s">
+        <v>1714</v>
+      </c>
       <c r="P482" t="s">
         <v>3452</v>
       </c>
@@ -48539,7 +48551,7 @@
         <v>72</v>
       </c>
       <c r="L485" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M485" t="s">
         <v>578</v>
@@ -48654,7 +48666,7 @@
         <v>72</v>
       </c>
       <c r="L487" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M487" t="s">
         <v>3489</v>
@@ -48719,7 +48731,7 @@
         <v>72</v>
       </c>
       <c r="L488" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M488" t="s">
         <v>578</v>
@@ -48781,7 +48793,7 @@
         <v>72</v>
       </c>
       <c r="L489" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M489" t="s">
         <v>125</v>
@@ -48849,7 +48861,7 @@
         <v>72</v>
       </c>
       <c r="L490" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M490" t="s">
         <v>125</v>
@@ -49218,7 +49230,7 @@
         <v>72</v>
       </c>
       <c r="L496" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M496" t="s">
         <v>578</v>
@@ -49280,7 +49292,7 @@
         <v>72</v>
       </c>
       <c r="L497" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M497" t="s">
         <v>125</v>
@@ -49351,7 +49363,7 @@
         <v>72</v>
       </c>
       <c r="L498" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M498" t="s">
         <v>125</v>
@@ -49605,7 +49617,7 @@
         <v>432</v>
       </c>
       <c r="L502" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M502" t="s">
         <v>3540</v>
@@ -49953,7 +49965,7 @@
         <v>72</v>
       </c>
       <c r="L508" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M508" t="s">
         <v>578</v>
@@ -50015,7 +50027,7 @@
         <v>72</v>
       </c>
       <c r="L509" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M509" t="s">
         <v>125</v>
@@ -50086,7 +50098,7 @@
         <v>72</v>
       </c>
       <c r="L510" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M510" t="s">
         <v>125</v>
@@ -50331,7 +50343,7 @@
         <v>432</v>
       </c>
       <c r="L514" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M514" t="s">
         <v>3540</v>
@@ -50514,7 +50526,7 @@
         <v>432</v>
       </c>
       <c r="L517" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M517" t="s">
         <v>3540</v>
@@ -50700,7 +50712,7 @@
         <v>72</v>
       </c>
       <c r="L520" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M520" t="s">
         <v>578</v>
@@ -50762,7 +50774,7 @@
         <v>72</v>
       </c>
       <c r="L521" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M521" t="s">
         <v>125</v>
@@ -50833,7 +50845,7 @@
         <v>72</v>
       </c>
       <c r="L522" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M522" t="s">
         <v>125</v>
@@ -51143,7 +51155,7 @@
         <v>432</v>
       </c>
       <c r="L527" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M527" t="s">
         <v>3540</v>
@@ -51267,7 +51279,7 @@
         <v>72</v>
       </c>
       <c r="L529" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M529" t="s">
         <v>578</v>
@@ -51329,7 +51341,7 @@
         <v>72</v>
       </c>
       <c r="L530" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M530" t="s">
         <v>125</v>
@@ -51397,7 +51409,7 @@
         <v>72</v>
       </c>
       <c r="L531" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M531" t="s">
         <v>125</v>
@@ -51810,7 +51822,7 @@
         <v>432</v>
       </c>
       <c r="L538" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M538" t="s">
         <v>3836</v>
@@ -52052,7 +52064,7 @@
         <v>72</v>
       </c>
       <c r="L542" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M542" t="s">
         <v>3863</v>
@@ -52176,7 +52188,7 @@
         <v>432</v>
       </c>
       <c r="L544" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M544" t="s">
         <v>3836</v>
@@ -52303,7 +52315,7 @@
         <v>432</v>
       </c>
       <c r="L546" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M546" t="s">
         <v>3891</v>
@@ -52430,7 +52442,7 @@
         <v>72</v>
       </c>
       <c r="L548" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M548" t="s">
         <v>578</v>
@@ -52492,7 +52504,7 @@
         <v>72</v>
       </c>
       <c r="L549" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M549" t="s">
         <v>125</v>
@@ -52557,7 +52569,7 @@
         <v>72</v>
       </c>
       <c r="L550" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M550" t="s">
         <v>125</v>
@@ -52622,7 +52634,7 @@
         <v>432</v>
       </c>
       <c r="L551" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M551" t="s">
         <v>3931</v>
@@ -53375,7 +53387,7 @@
         <v>72</v>
       </c>
       <c r="L563" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M563" t="s">
         <v>578</v>
@@ -53437,7 +53449,7 @@
         <v>72</v>
       </c>
       <c r="L564" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M564" t="s">
         <v>125</v>
@@ -53788,7 +53800,7 @@
         <v>72</v>
       </c>
       <c r="L570" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M570" t="s">
         <v>423</v>
@@ -55771,7 +55783,7 @@
         <v>432</v>
       </c>
       <c r="L600" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M600" t="s">
         <v>4233</v>
@@ -56303,7 +56315,7 @@
         <v>72</v>
       </c>
       <c r="L608" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M608" t="s">
         <v>125</v>
@@ -56424,7 +56436,7 @@
         <v>72</v>
       </c>
       <c r="L610" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M610" t="s">
         <v>125</v>
@@ -56542,7 +56554,7 @@
         <v>72</v>
       </c>
       <c r="L612" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M612" t="s">
         <v>578</v>
@@ -56604,7 +56616,7 @@
         <v>28</v>
       </c>
       <c r="L613" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="Q613" t="s">
         <v>567</v>
@@ -56666,7 +56678,7 @@
         <v>72</v>
       </c>
       <c r="L614" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M614" t="s">
         <v>4321</v>
@@ -56846,7 +56858,7 @@
         <v>72</v>
       </c>
       <c r="L617" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M617" t="s">
         <v>125</v>
@@ -57404,7 +57416,7 @@
         <v>72</v>
       </c>
       <c r="L626" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M626" t="s">
         <v>125</v>
@@ -57466,7 +57478,7 @@
         <v>72</v>
       </c>
       <c r="L627" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M627" t="s">
         <v>125</v>
@@ -57528,7 +57540,7 @@
         <v>72</v>
       </c>
       <c r="L628" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M628" t="s">
         <v>125</v>
@@ -57590,7 +57602,7 @@
         <v>72</v>
       </c>
       <c r="L629" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M629" t="s">
         <v>125</v>
@@ -57652,7 +57664,7 @@
         <v>72</v>
       </c>
       <c r="L630" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M630" t="s">
         <v>125</v>
@@ -57714,7 +57726,7 @@
         <v>72</v>
       </c>
       <c r="L631" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M631" t="s">
         <v>125</v>
@@ -57776,7 +57788,7 @@
         <v>72</v>
       </c>
       <c r="L632" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M632" t="s">
         <v>125</v>
@@ -57838,7 +57850,7 @@
         <v>72</v>
       </c>
       <c r="L633" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M633" t="s">
         <v>125</v>
@@ -57900,7 +57912,7 @@
         <v>72</v>
       </c>
       <c r="L634" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M634" t="s">
         <v>125</v>
@@ -57962,7 +57974,7 @@
         <v>72</v>
       </c>
       <c r="L635" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M635" t="s">
         <v>125</v>
@@ -58024,7 +58036,7 @@
         <v>72</v>
       </c>
       <c r="L636" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M636" t="s">
         <v>125</v>
@@ -58086,7 +58098,7 @@
         <v>72</v>
       </c>
       <c r="L637" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M637" t="s">
         <v>125</v>
@@ -58148,7 +58160,7 @@
         <v>72</v>
       </c>
       <c r="L638" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M638" t="s">
         <v>125</v>
@@ -58266,7 +58278,7 @@
         <v>72</v>
       </c>
       <c r="L640" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M640" t="s">
         <v>125</v>
@@ -58331,7 +58343,7 @@
         <v>432</v>
       </c>
       <c r="L641" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M641" t="s">
         <v>4501</v>
@@ -58399,7 +58411,7 @@
         <v>72</v>
       </c>
       <c r="L642" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M642" t="s">
         <v>557</v>
@@ -58461,7 +58473,7 @@
         <v>72</v>
       </c>
       <c r="L643" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M643" t="s">
         <v>125</v>
@@ -58523,7 +58535,7 @@
         <v>72</v>
       </c>
       <c r="L644" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M644" t="s">
         <v>578</v>
@@ -58972,7 +58984,7 @@
         <v>432</v>
       </c>
       <c r="L651" t="s">
-        <v>5731</v>
+        <v>5730</v>
       </c>
       <c r="M651" t="s">
         <v>4578</v>
@@ -59235,7 +59247,7 @@
         <v>432</v>
       </c>
       <c r="L655" t="s">
-        <v>5731</v>
+        <v>5730</v>
       </c>
       <c r="M655" t="s">
         <v>4609</v>
@@ -60030,7 +60042,7 @@
         <v>72</v>
       </c>
       <c r="L667" t="s">
-        <v>5731</v>
+        <v>5730</v>
       </c>
       <c r="M667" t="s">
         <v>4700</v>
@@ -60219,7 +60231,7 @@
         <v>72</v>
       </c>
       <c r="L670" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M670" t="s">
         <v>125</v>
@@ -60284,7 +60296,7 @@
         <v>432</v>
       </c>
       <c r="L671" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M671" t="s">
         <v>125</v>
@@ -60473,7 +60485,7 @@
         <v>432</v>
       </c>
       <c r="L674" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M674" t="s">
         <v>4750</v>
@@ -60541,7 +60553,7 @@
         <v>432</v>
       </c>
       <c r="L675" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M675" t="s">
         <v>4759</v>
@@ -60733,7 +60745,7 @@
         <v>432</v>
       </c>
       <c r="L678" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M678" t="s">
         <v>4779</v>
@@ -60801,7 +60813,7 @@
         <v>432</v>
       </c>
       <c r="L679" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M679" t="s">
         <v>4788</v>
@@ -60869,7 +60881,7 @@
         <v>432</v>
       </c>
       <c r="L680" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M680" t="s">
         <v>4797</v>
@@ -60934,7 +60946,7 @@
         <v>432</v>
       </c>
       <c r="L681" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M681" t="s">
         <v>125</v>
@@ -61055,7 +61067,7 @@
         <v>72</v>
       </c>
       <c r="L683" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M683" t="s">
         <v>578</v>
@@ -61235,7 +61247,7 @@
         <v>72</v>
       </c>
       <c r="L686" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M686" t="s">
         <v>125</v>
@@ -61303,7 +61315,7 @@
         <v>72</v>
       </c>
       <c r="L687" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M687" t="s">
         <v>125</v>
@@ -61542,7 +61554,7 @@
         <v>72</v>
       </c>
       <c r="L691" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M691" t="s">
         <v>125</v>
@@ -61610,7 +61622,7 @@
         <v>72</v>
       </c>
       <c r="L692" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M692" t="s">
         <v>125</v>
@@ -62059,7 +62071,7 @@
         <v>72</v>
       </c>
       <c r="L699" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M699" t="s">
         <v>125</v>
@@ -62519,7 +62531,7 @@
         <v>72</v>
       </c>
       <c r="L707" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M707" t="s">
         <v>125</v>
@@ -62581,7 +62593,7 @@
         <v>72</v>
       </c>
       <c r="L708" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M708" t="s">
         <v>125</v>
@@ -62702,7 +62714,7 @@
         <v>72</v>
       </c>
       <c r="L710" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M710" t="s">
         <v>125</v>
@@ -62767,7 +62779,7 @@
         <v>72</v>
       </c>
       <c r="L711" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M711" t="s">
         <v>125</v>
@@ -62891,7 +62903,7 @@
         <v>72</v>
       </c>
       <c r="L713" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M713" t="s">
         <v>125</v>
@@ -63021,7 +63033,7 @@
         <v>72</v>
       </c>
       <c r="L715" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M715" t="s">
         <v>125</v>
@@ -63210,7 +63222,7 @@
         <v>72</v>
       </c>
       <c r="L718" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M718" t="s">
         <v>125</v>
@@ -63278,7 +63290,7 @@
         <v>72</v>
       </c>
       <c r="L719" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M719" t="s">
         <v>125</v>
@@ -63532,7 +63544,7 @@
         <v>72</v>
       </c>
       <c r="L723" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M723" t="s">
         <v>125</v>
@@ -63600,7 +63612,7 @@
         <v>72</v>
       </c>
       <c r="L724" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M724" t="s">
         <v>125</v>
@@ -63724,7 +63736,7 @@
         <v>72</v>
       </c>
       <c r="L726" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M726" t="s">
         <v>578</v>
@@ -63786,7 +63798,7 @@
         <v>28</v>
       </c>
       <c r="L727" t="s">
-        <v>180</v>
+        <v>1714</v>
       </c>
       <c r="Q727" t="s">
         <v>567</v>
@@ -64019,7 +64031,7 @@
         <v>72</v>
       </c>
       <c r="L731" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M731" t="s">
         <v>125</v>
@@ -64143,7 +64155,7 @@
         <v>72</v>
       </c>
       <c r="L733" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M733" t="s">
         <v>125</v>
@@ -64270,7 +64282,7 @@
         <v>72</v>
       </c>
       <c r="L735" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M735" t="s">
         <v>125</v>
@@ -64397,7 +64409,7 @@
         <v>72</v>
       </c>
       <c r="L737" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M737" t="s">
         <v>125</v>
@@ -64524,7 +64536,7 @@
         <v>72</v>
       </c>
       <c r="L739" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M739" t="s">
         <v>125</v>
@@ -64651,7 +64663,7 @@
         <v>72</v>
       </c>
       <c r="L741" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M741" t="s">
         <v>125</v>
@@ -64778,7 +64790,7 @@
         <v>72</v>
       </c>
       <c r="L743" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M743" t="s">
         <v>125</v>
@@ -64905,7 +64917,7 @@
         <v>72</v>
       </c>
       <c r="L745" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M745" t="s">
         <v>125</v>
@@ -65032,7 +65044,7 @@
         <v>72</v>
       </c>
       <c r="L747" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M747" t="s">
         <v>125</v>
@@ -65159,7 +65171,7 @@
         <v>72</v>
       </c>
       <c r="L749" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M749" t="s">
         <v>125</v>
@@ -65227,7 +65239,7 @@
         <v>72</v>
       </c>
       <c r="L750" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M750" t="s">
         <v>125</v>
@@ -65590,7 +65602,7 @@
         <v>72</v>
       </c>
       <c r="L756" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M756" t="s">
         <v>5332</v>
@@ -65776,7 +65788,7 @@
         <v>72</v>
       </c>
       <c r="L759" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M759" t="s">
         <v>125</v>
@@ -65844,7 +65856,7 @@
         <v>432</v>
       </c>
       <c r="L760" t="s">
-        <v>5728</v>
+        <v>5730</v>
       </c>
       <c r="M760" t="s">
         <v>5358</v>
@@ -65971,7 +65983,7 @@
         <v>72</v>
       </c>
       <c r="L762" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M762" t="s">
         <v>125</v>
@@ -66098,7 +66110,7 @@
         <v>72</v>
       </c>
       <c r="L764" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M764" t="s">
         <v>125</v>
@@ -66225,7 +66237,7 @@
         <v>72</v>
       </c>
       <c r="L766" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M766" t="s">
         <v>578</v>
@@ -66287,7 +66299,7 @@
         <v>72</v>
       </c>
       <c r="L767" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M767" t="s">
         <v>5411</v>
@@ -66482,7 +66494,7 @@
         <v>72</v>
       </c>
       <c r="L770" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M770" t="s">
         <v>125</v>
@@ -66606,7 +66618,7 @@
         <v>72</v>
       </c>
       <c r="L772" t="s">
-        <v>5728</v>
+        <v>36</v>
       </c>
       <c r="M772" t="s">
         <v>5450</v>
@@ -66733,7 +66745,7 @@
         <v>72</v>
       </c>
       <c r="L774" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M774" t="s">
         <v>578</v>
@@ -66854,7 +66866,7 @@
         <v>432</v>
       </c>
       <c r="L776" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M776" t="s">
         <v>5481</v>
@@ -67152,7 +67164,7 @@
         <v>72</v>
       </c>
       <c r="L781" t="s">
-        <v>5728</v>
+        <v>49</v>
       </c>
       <c r="M781" t="s">
         <v>578</v>

</xml_diff>